<commit_message>
Use Cases reworked, FBM States
</commit_message>
<xml_diff>
--- a/work/Glossar.xlsx
+++ b/work/Glossar.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Benutzer 1\Meine Dateien\Uni\ESEP\SE2-Projekt\work\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96688A6-9167-480C-8F74-0DADD047EA48}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$Z$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$9</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Begriff</t>
   </si>
@@ -74,70 +84,402 @@
   </si>
   <si>
     <t>Werkstück mit Bohrung ohne Metalleinsatz</t>
+  </si>
+  <si>
+    <t>LB_Start</t>
+  </si>
+  <si>
+    <t>LB_Switch</t>
+  </si>
+  <si>
+    <t>LB_Ramp</t>
+  </si>
+  <si>
+    <t>LB_End</t>
+  </si>
+  <si>
+    <t>Lichtschranke am Anfang des Förderbandes</t>
+  </si>
+  <si>
+    <t>Lichtschranke an der Weiche</t>
+  </si>
+  <si>
+    <t>Lichtschranke an der Rutsche</t>
+  </si>
+  <si>
+    <t>Lichtschranke am Ende des Förderbandes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="40.43"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -145,7 +487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -153,7 +495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -161,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -169,7 +511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -177,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -185,7 +527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="26.25">
+    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -193,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -201,7 +543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -209,7 +551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -217,8 +559,40 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$Z$9"/>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:Z9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>